<commit_message>
Update carga datos Valentina Close to Open.xlsx
</commit_message>
<xml_diff>
--- a/carga datos Valentina Close to Open.xlsx
+++ b/carga datos Valentina Close to Open.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valentina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Thinkpad E14\Documents\GitHub\Arkad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F980A12A-4488-405E-8845-5E898054AE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41839E38-4F69-4674-ABB6-1DAE72B95870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -85,13 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D371" sqref="D371"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="A374" sqref="A374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3358,7 +3356,7 @@
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A370" s="3">
+      <c r="A370" s="2">
         <v>45491</v>
       </c>
       <c r="B370">

</xml_diff>

<commit_message>
Upload file carga datos históricos Algoritmo Valentina Open to Close
</commit_message>
<xml_diff>
--- a/carga datos Valentina Close to Open.xlsx
+++ b/carga datos Valentina Close to Open.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Thinkpad E14\Documents\GitHub\Arkad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41839E38-4F69-4674-ABB6-1DAE72B95870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A84D8-1BF4-44EE-B9E9-E070F5432F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B370"/>
+  <dimension ref="A1:B378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="A374" sqref="A374"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="A373" sqref="A373:A378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3363,6 +3363,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371" s="2">
+        <v>45492</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372" s="2">
+        <v>45493</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373" s="2">
+        <v>45494</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374" s="2">
+        <v>45495</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375" s="2">
+        <v>45496</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376" s="2">
+        <v>45497</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377" s="2">
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378" s="2">
+        <v>45499</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>